<commit_message>
tweaked formatting of numbers
</commit_message>
<xml_diff>
--- a/extras/demo.xlsx
+++ b/extras/demo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gforeman/Documents/workspace_mars/numcheck/extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gforeman/git/numcheck/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="3960" yWindow="3180" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,10 +350,13 @@
   <dimension ref="C1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
@@ -365,12 +368,12 @@
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2">
-        <v>12345</v>
+        <v>2949444438</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3">
-        <v>67890</v>
+        <v>3949444438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
for loop with if statements, odd and even check
</commit_message>
<xml_diff>
--- a/extras/demo.xlsx
+++ b/extras/demo.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gforeman/git/numcheck/extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olzhas.shaikenov/git/numcheck/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="3180" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Number</t>
   </si>
   <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>Response</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>23s3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,15 +357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D3"/>
+  <dimension ref="C1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.2">
@@ -363,17 +373,41 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2">
-        <v>2949444438</v>
+        <v>222222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>3949444438</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>22222</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel fixes and improved test case
</commit_message>
<xml_diff>
--- a/extras/demo.xlsx
+++ b/extras/demo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olzhas.shaikenov/git/numcheck/extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gforeman/git/numcheck/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,29 +27,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Number</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>23s3</t>
+    <t>Is in DB?</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>a column</t>
+  </si>
+  <si>
+    <t>b column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,57 +359,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D27"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="C2">
-        <v>222222</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
+        <v>2949444438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>3949444438</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C11">
-        <v>22222</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>3949444438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>3949444438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>3949444438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>3949444438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>3949444438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>3949444438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated documentation, minor mods
</commit_message>
<xml_diff>
--- a/extras/demo.xlsx
+++ b/extras/demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gforeman/git/numcheck/extras/"/>
     </mc:Choice>
@@ -27,13 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Is in DB?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>aaa</t>
   </si>
@@ -41,17 +35,21 @@
     <t>bbbb</t>
   </si>
   <si>
-    <t>a column</t>
+    <t>2949444438</t>
   </si>
   <si>
-    <t>b column</t>
+    <t>3949444438</t>
+  </si>
+  <si>
+    <t>1111111111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -359,75 +357,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+      <selection activeCell="D9" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2949444438</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>3949444438</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>1111111111</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>2949444438</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C3">
-        <v>3949444438</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>3949444438</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>3949444438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>3949444438</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>3949444438</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>3949444438</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>3949444438</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <v>3949444438</v>
+      <c r="D9" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>